<commit_message>
bug posición archivo excel
</commit_message>
<xml_diff>
--- a/assets/docs/requisicion_personal.xlsx
+++ b/assets/docs/requisicion_personal.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Nombre de la Empresa solicitante y/o cliente:</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">Ubicación física del recurso (dirección cliente si aplica): </t>
   </si>
   <si>
-    <t>Nombre del Puesto:</t>
-  </si>
-  <si>
     <t>Número de vacantes:</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Solicitante</t>
   </si>
   <si>
-    <t>Posición</t>
-  </si>
-  <si>
     <t>Área</t>
   </si>
   <si>
@@ -131,6 +125,9 @@
   </si>
   <si>
     <t>Folio</t>
+  </si>
+  <si>
+    <t>Posición:</t>
   </si>
 </sst>
 </file>
@@ -254,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -304,21 +301,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -367,32 +349,6 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -484,7 +440,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -498,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -534,173 +490,164 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1125,12 +1072,12 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="72" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="4" customWidth="1"/>
@@ -1142,409 +1089,407 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="30" t="s">
+      <c r="A1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="73"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="50"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="19" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="53"/>
+    </row>
+    <row r="10" spans="1:7" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="66"/>
-    </row>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
-    </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="58"/>
-    </row>
-    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="68" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
+    </row>
+    <row r="12" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
-    </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="67"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
-    </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
-    </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
-    </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-    </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="43"/>
-    </row>
-    <row r="12" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="68" t="s">
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="69"/>
+    </row>
+    <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:24" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="38"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="43"/>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-    </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="35"/>
-    </row>
-    <row r="18" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="I18" s="18"/>
-    </row>
-    <row r="19" spans="1:24" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="61"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="72"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="72"/>
     </row>
     <row r="22" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="68" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
+      <c r="A22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="62"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="R22" s="15"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
+      <c r="S22" s="70"/>
+      <c r="T22" s="70"/>
       <c r="U22" s="15"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
+      <c r="V22" s="70"/>
+      <c r="W22" s="70"/>
+      <c r="X22" s="70"/>
     </row>
     <row r="23" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
+      <c r="A23" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="62"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="12"/>
       <c r="R23" s="15"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
       <c r="U23" s="15"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
+      <c r="V23" s="70"/>
+      <c r="W23" s="70"/>
+      <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="62"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="64"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="70"/>
+      <c r="T24" s="70"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="70"/>
+      <c r="W24" s="70"/>
+      <c r="X24" s="70"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="62"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="64"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="70"/>
+      <c r="T25" s="70"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="70"/>
+      <c r="W25" s="70"/>
+      <c r="X25" s="70"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="21"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="68" t="s">
+      <c r="B26" s="62"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="70"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="70"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="70"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="62"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="64"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="70"/>
+      <c r="T27" s="70"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="70"/>
+      <c r="W27" s="70"/>
+      <c r="X27" s="70"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A28" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="61"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="70"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="70"/>
+      <c r="W28" s="70"/>
+      <c r="X28" s="70"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="62"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="64"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="70"/>
+      <c r="T29" s="70"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="70"/>
+      <c r="W29" s="70"/>
+      <c r="X29" s="70"/>
+    </row>
+    <row r="30" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="21"/>
-      <c r="W25" s="21"/>
-      <c r="X25" s="21"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A26" s="68" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="27"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A27" s="68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="27"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="21"/>
-      <c r="W27" s="21"/>
-      <c r="X27" s="21"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="21"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="21"/>
-      <c r="W29" s="21"/>
-      <c r="X29" s="21"/>
-    </row>
-    <row r="30" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="68" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="27"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="12"/>
       <c r="R30" s="15"/>
       <c r="S30" s="17"/>
@@ -1555,93 +1500,93 @@
       <c r="X30" s="16"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="62"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="64"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="70"/>
+      <c r="T31" s="70"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="70"/>
+      <c r="W31" s="70"/>
+      <c r="X31" s="70"/>
+    </row>
+    <row r="32" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="62"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="64"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="70"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="70"/>
+      <c r="W32" s="70"/>
+      <c r="X32" s="70"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="70"/>
+      <c r="T33" s="70"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="70"/>
+      <c r="W33" s="70"/>
+      <c r="X33" s="70"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A34" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="21"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="21"/>
-    </row>
-    <row r="32" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="21"/>
-      <c r="W32" s="21"/>
-      <c r="X32" s="21"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A33" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="21"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A34" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="64"/>
       <c r="R34" s="14"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
       <c r="U34" s="15"/>
-      <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="21"/>
+      <c r="V34" s="70"/>
+      <c r="W34" s="70"/>
+      <c r="X34" s="70"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="R35" s="14"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
+      <c r="S35" s="70"/>
+      <c r="T35" s="70"/>
       <c r="U35" s="15"/>
-      <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
-      <c r="X35" s="21"/>
+      <c r="V35" s="70"/>
+      <c r="W35" s="70"/>
+      <c r="X35" s="70"/>
     </row>
     <row r="36" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="73"/>
+      <c r="A36" s="26"/>
       <c r="D36" s="3"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="74"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1650,7 +1595,7 @@
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:24" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="75"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1659,7 +1604,7 @@
       <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:24" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="76"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -1668,7 +1613,7 @@
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A40" s="74"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -1677,35 +1622,23 @@
       <c r="G40" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G16"/>
+  <mergeCells count="61">
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="V34:X34"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="V35:X35"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="V32:X32"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="V33:X33"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="V31:X31"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="B30:G30"/>
     <mergeCell ref="B34:G34"/>
     <mergeCell ref="S22:T22"/>
     <mergeCell ref="S23:T23"/>
@@ -1722,24 +1655,35 @@
     <mergeCell ref="V26:X26"/>
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="V27:X27"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="B29:G29"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="V31:X31"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="V34:X34"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="V35:X35"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="V32:X32"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="V33:X33"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.59055118110236227" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.39370078740157483"/>

</xml_diff>